<commit_message>
update documentation, add map.
</commit_message>
<xml_diff>
--- a/Documentation/Описание структуры проекта.xlsx
+++ b/Documentation/Описание структуры проекта.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AF26E8-026C-4961-BE2B-A95F17D13AA6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F560A01-511E-42C4-A485-6496DEACF1E2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Имя еденицы</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Под объектом понимается, то что хранится в проперти data и то что рендерится на карту</t>
   </si>
   <si>
-    <t>В слое в metadata хранится: {parentLayers: [], childLayers: [], elements: []}</t>
-  </si>
-  <si>
     <t>parentLayers - список слоев которым пренадлежит данный. Данный слой может быть показан, только если все родительские слои видны</t>
   </si>
   <si>
@@ -61,13 +58,22 @@
     <t>year - год когда появится этот объект, необходимо для фильтриции</t>
   </si>
   <si>
-    <t>В объектах в properties хранятся данные для фильтрации: .{ ownerLayer : "", ownerElement: "" ,  year: ""}</t>
-  </si>
-  <si>
     <t>ownerLayer - id слоя владельца</t>
   </si>
   <si>
     <t>ownerElement - id элемента, который хранится в слое layer</t>
+  </si>
+  <si>
+    <t>В объектах в properties хранятся данные для фильтрации: .{ ownerLayer : "", ownerElement: "" ,  year: "", popupData : {}}</t>
+  </si>
+  <si>
+    <t>popupData - данные для отображения всплывающего окна при нажатии</t>
+  </si>
+  <si>
+    <t>В слое в metadata хранится: {parentLayers: [], childLayers: [], elements: [], popupHtml: ""}</t>
+  </si>
+  <si>
+    <t>popupHtml: html модель всплывающего окна, с кнокаутовским датабинденгом</t>
   </si>
 </sst>
 </file>
@@ -388,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,12 +407,13 @@
     <col min="3" max="3" width="84.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="41" style="1" customWidth="1"/>
     <col min="5" max="5" width="37.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="55.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="57.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="37.5703125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="46.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -425,43 +432,49 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>12</v>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>